<commit_message>
Update Charging Profile Temp Current Voltage Ranges.xlsx
</commit_message>
<xml_diff>
--- a/Charging Profile Temp Current Voltage Ranges.xlsx
+++ b/Charging Profile Temp Current Voltage Ranges.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab8d326e7f61b561/Documents/GitHub/Alpha-BMS-SW-HW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6981D5EE-F0AE-4CBF-8156-BC94CCE5B05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{6981D5EE-F0AE-4CBF-8156-BC94CCE5B05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3582235D-A5CD-4BFD-877D-758C10B2FED1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{E4DCD1D3-DDF6-4162-95EA-A66D5D77108B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{E4DCD1D3-DDF6-4162-95EA-A66D5D77108B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Beta Charger Test Values" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>Voltage 1</t>
   </si>
@@ -107,6 +108,27 @@
   </si>
   <si>
     <t>Temp Deg</t>
+  </si>
+  <si>
+    <t>0-9</t>
+  </si>
+  <si>
+    <t>25-44</t>
+  </si>
+  <si>
+    <t>10-24</t>
+  </si>
+  <si>
+    <t>Temp Range</t>
+  </si>
+  <si>
+    <t>45-47</t>
+  </si>
+  <si>
+    <t>48-54</t>
+  </si>
+  <si>
+    <t>55&gt;</t>
   </si>
 </sst>
 </file>
@@ -130,7 +152,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +162,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -170,7 +216,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -188,6 +261,14 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -489,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0587C16C-28E3-4773-83CF-78CCE8615A87}">
   <dimension ref="D4:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,10 +625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B62F513-D9A2-4954-8D27-7470F5B66003}">
-  <dimension ref="A7:I12"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -557,28 +638,82 @@
     <col min="4" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D1" s="8"/>
+    </row>
+    <row r="4" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -586,74 +721,78 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
         <v>10</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>11</v>
+      <c r="F8" s="7">
+        <v>25</v>
+      </c>
+      <c r="G8" s="8">
+        <v>45</v>
+      </c>
+      <c r="H8" s="9">
+        <v>48</v>
+      </c>
+      <c r="I8" s="10">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1">
-        <v>25</v>
-      </c>
-      <c r="G9" s="1">
-        <v>45</v>
-      </c>
-      <c r="H9" s="1">
-        <v>50</v>
-      </c>
-      <c r="I9" s="1">
-        <v>60</v>
+        <v>22</v>
+      </c>
+      <c r="D9" s="8">
+        <v>4150</v>
+      </c>
+      <c r="E9" s="7">
+        <v>4200</v>
+      </c>
+      <c r="F9" s="7">
+        <v>4200</v>
+      </c>
+      <c r="G9" s="8">
+        <v>4200</v>
+      </c>
+      <c r="H9" s="9">
+        <v>4100</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1">
-        <v>4150</v>
-      </c>
-      <c r="E10" s="1">
-        <v>4200</v>
-      </c>
-      <c r="F10" s="1">
-        <v>4200</v>
-      </c>
-      <c r="G10" s="1">
-        <v>4200</v>
-      </c>
-      <c r="H10" s="1">
-        <v>4100</v>
-      </c>
-      <c r="I10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>6000</v>
+      </c>
+      <c r="F10" s="7">
+        <v>6000</v>
+      </c>
+      <c r="G10" s="8">
+        <v>3000</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1000</v>
+      </c>
+      <c r="I10" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -662,60 +801,244 @@
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="8">
         <v>1000</v>
       </c>
-      <c r="E11" s="1">
-        <v>6000</v>
-      </c>
-      <c r="F11" s="1">
-        <v>6000</v>
-      </c>
-      <c r="G11" s="1">
-        <v>6000</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="E11" s="7">
+        <v>3000</v>
+      </c>
+      <c r="F11" s="7">
+        <v>3000</v>
+      </c>
+      <c r="G11" s="8">
         <v>1000</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="H11" s="9">
         <v>1000</v>
       </c>
-      <c r="E12" s="1">
-        <v>3000</v>
-      </c>
-      <c r="F12" s="1">
-        <v>3000</v>
-      </c>
-      <c r="G12" s="1">
-        <v>3000</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1000</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="I11" s="10" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E6" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3372743A-A51F-4567-8EAE-B91200DF5E9F}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="17.1796875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D1" s="8"/>
+    </row>
+    <row r="4" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7">
+        <v>25</v>
+      </c>
+      <c r="G8" s="8">
+        <v>45</v>
+      </c>
+      <c r="H8" s="9">
+        <v>48</v>
+      </c>
+      <c r="I8" s="10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="8">
+        <v>4150</v>
+      </c>
+      <c r="E9" s="7">
+        <v>4200</v>
+      </c>
+      <c r="F9" s="7">
+        <v>4200</v>
+      </c>
+      <c r="G9" s="8">
+        <v>4200</v>
+      </c>
+      <c r="H9" s="9">
+        <v>4100</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>6000</v>
+      </c>
+      <c r="F10" s="7">
+        <v>6000</v>
+      </c>
+      <c r="G10" s="8">
+        <v>3000</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1000</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="7">
+        <v>6000</v>
+      </c>
+      <c r="F11" s="7">
+        <v>6000</v>
+      </c>
+      <c r="G11" s="8">
+        <v>3000</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1000</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E6" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major Update: 5th Dec 2024
Major Temperature Ranges & Voltage Ranges
Advanced Charging Algorithm: Voltage & Current,
End Voltage : 2300mV, 9200mV,
TS Sensors CTEMP, FTEMP, TS2& TS3 Selection,
Updated Values & Added Auto Recovery for OCC & OCD Protections
Updated ZVCHG PRECHG, CUV, CUVC
Updated OTC, OTD, OTF, UTC, UTD
</commit_message>
<xml_diff>
--- a/Charging Profile Temp Current Voltage Ranges.xlsx
+++ b/Charging Profile Temp Current Voltage Ranges.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab8d326e7f61b561/Documents/GitHub/Alpha-BMS-SW-HW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Rohit Cluttered\Alpha BQ BMS SW HW\Alpha-BMS-SW-HW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{6981D5EE-F0AE-4CBF-8156-BC94CCE5B05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3582235D-A5CD-4BFD-877D-758C10B2FED1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{E4DCD1D3-DDF6-4162-95EA-A66D5D77108B}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11625" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Beta Charger Test Values" sheetId="4" r:id="rId3"/>
+    <sheet name="Updated Values 5th Dec 24" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="52">
   <si>
     <t>Voltage 1</t>
   </si>
@@ -129,12 +129,66 @@
   </si>
   <si>
     <t>55&gt;</t>
+  </si>
+  <si>
+    <t>4S5P / 4S6P</t>
+  </si>
+  <si>
+    <t>4S2P / 4S3P</t>
+  </si>
+  <si>
+    <t>Temp Range °</t>
+  </si>
+  <si>
+    <t>0-9°</t>
+  </si>
+  <si>
+    <t>10-24°</t>
+  </si>
+  <si>
+    <t>25-44°</t>
+  </si>
+  <si>
+    <t>48-54°</t>
+  </si>
+  <si>
+    <t>45-47°</t>
+  </si>
+  <si>
+    <t>55°&gt;</t>
+  </si>
+  <si>
+    <t>V150</t>
+  </si>
+  <si>
+    <t>V90</t>
+  </si>
+  <si>
+    <t>PRECHG</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>MED</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>ZVCHG</t>
+  </si>
+  <si>
+    <t>25-39</t>
+  </si>
+  <si>
+    <t>40-47</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +243,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -202,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -244,6 +304,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -567,16 +633,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0587C16C-28E3-4773-83CF-78CCE8615A87}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:H6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -590,7 +656,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>1</v>
       </c>
@@ -604,7 +670,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>2</v>
       </c>
@@ -624,25 +690,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B62F513-D9A2-4954-8D27-7470F5B66003}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="17.1796875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D1" s="8"/>
     </row>
-    <row r="4" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
@@ -667,7 +734,214 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>10</v>
+      </c>
+      <c r="F8" s="7">
+        <v>25</v>
+      </c>
+      <c r="G8" s="8">
+        <v>45</v>
+      </c>
+      <c r="H8" s="9">
+        <v>48</v>
+      </c>
+      <c r="I8" s="10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="8">
+        <v>4150</v>
+      </c>
+      <c r="E9" s="7">
+        <v>4200</v>
+      </c>
+      <c r="F9" s="7">
+        <v>4200</v>
+      </c>
+      <c r="G9" s="8">
+        <v>4200</v>
+      </c>
+      <c r="H9" s="9">
+        <v>4100</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>6000</v>
+      </c>
+      <c r="F10" s="7">
+        <v>6000</v>
+      </c>
+      <c r="G10" s="8">
+        <v>3000</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1000</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3000</v>
+      </c>
+      <c r="F11" s="7">
+        <v>3000</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1000</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.7109375" style="1"/>
+    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D1" s="8"/>
+    </row>
+    <row r="4" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -692,7 +966,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
@@ -717,7 +991,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
@@ -742,7 +1016,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -767,7 +1041,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -796,7 +1070,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -810,13 +1084,13 @@
         <v>1000</v>
       </c>
       <c r="E11" s="7">
+        <v>6000</v>
+      </c>
+      <c r="F11" s="7">
+        <v>6000</v>
+      </c>
+      <c r="G11" s="8">
         <v>3000</v>
-      </c>
-      <c r="F11" s="7">
-        <v>3000</v>
-      </c>
-      <c r="G11" s="8">
-        <v>1000</v>
       </c>
       <c r="H11" s="9">
         <v>1000</v>
@@ -833,26 +1107,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3372743A-A51F-4567-8EAE-B91200DF5E9F}">
-  <dimension ref="A1:I11"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F12" sqref="E12:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="17.1796875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="2" width="8.7109375" style="1"/>
+    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D1" s="8"/>
-    </row>
-    <row r="4" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
@@ -877,7 +1148,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -890,10 +1161,10 @@
         <v>29</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>32</v>
@@ -902,7 +1173,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
@@ -911,13 +1182,13 @@
       <c r="D7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="12" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="13" t="s">
@@ -927,7 +1198,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
@@ -936,23 +1207,23 @@
       <c r="D8" s="8">
         <v>0</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="16">
         <v>10</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="16">
         <v>25</v>
       </c>
-      <c r="G8" s="8">
-        <v>45</v>
+      <c r="G8" s="7">
+        <v>40</v>
       </c>
       <c r="H8" s="9">
         <v>48</v>
       </c>
       <c r="I8" s="10">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -961,13 +1232,13 @@
       <c r="D9" s="8">
         <v>4150</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="16">
         <v>4200</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="16">
         <v>4200</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>4200</v>
       </c>
       <c r="H9" s="9">
@@ -977,7 +1248,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -990,13 +1261,13 @@
       <c r="D10" s="8">
         <v>1000</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="16">
         <v>6000</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="16">
         <v>6000</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>3000</v>
       </c>
       <c r="H10" s="9">
@@ -1006,12 +1277,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>23</v>
@@ -1019,13 +1290,13 @@
       <c r="D11" s="8">
         <v>1000</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="16">
         <v>6000</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="16">
         <v>6000</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>3000</v>
       </c>
       <c r="H11" s="9">
@@ -1035,10 +1306,107 @@
         <v>21</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="16">
+        <v>3000</v>
+      </c>
+      <c r="F12" s="16">
+        <v>3000</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1000</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1000</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2500</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G15" s="1">
+        <v>3600</v>
+      </c>
+      <c r="H15" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="E6" twoDigitTextYear="1"/>
-  </ignoredErrors>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>